<commit_message>
Removing un-used imports, etc
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>testcasename</t>
   </si>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +426,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>